<commit_message>
removed rrexp[Rule*Expression] from formalampersand. It is the same as term[Rule*Expression]
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/AST.xlsx
+++ b/AmpersandData/FormalAmpersand/AST.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\hjo20125\Git\ampersand\ampersandData\FormalAmpersand\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="-15" windowWidth="7470" windowHeight="4965" tabRatio="870" activeTab="3"/>
+    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -343,9 +348,6 @@
   </si>
   <si>
     <t>relations~</t>
-  </si>
-  <si>
-    <t>rrexp</t>
   </si>
   <si>
     <t>rrmean</t>
@@ -414,6 +416,9 @@
       </rPr>
       <t>]</t>
     </r>
+  </si>
+  <si>
+    <t>term</t>
   </si>
 </sst>
 </file>
@@ -469,6 +474,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -516,7 +524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,7 +559,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -766,9 +774,9 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -785,7 +793,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -802,7 +810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -810,13 +818,13 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -824,7 +832,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
@@ -841,20 +849,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -876,9 +884,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -886,7 +894,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -907,7 +915,7 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -919,12 +927,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -932,7 +940,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -951,9 +959,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -961,7 +969,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -980,9 +988,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -990,7 +998,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1009,9 +1017,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1019,7 +1027,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1040,9 +1048,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1050,19 +1058,19 @@
         <v>97</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
       <c r="F1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1095,20 +1103,20 @@
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1132,9 +1140,9 @@
       <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1151,10 +1159,10 @@
         <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1187,9 +1195,9 @@
       <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1206,10 +1214,10 @@
         <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1229,7 +1237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1249,21 +1257,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1285,9 +1293,9 @@
       <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1295,7 +1303,7 @@
         <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
@@ -1313,7 +1321,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1348,11 +1356,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1420,16 +1430,16 @@
         <v>81</v>
       </c>
       <c r="W1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="Y1" t="s">
         <v>84</v>
       </c>
       <c r="Z1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA1" t="s">
         <v>99</v>
@@ -1447,13 +1457,13 @@
         <v>97</v>
       </c>
       <c r="AF1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AG1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1565,9 +1575,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1578,7 +1588,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1600,9 +1610,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1616,7 +1626,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1643,9 +1653,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1653,7 +1663,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Some work on interface of RAP
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/AST.xlsx
+++ b/AmpersandData/FormalAmpersand/AST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" activeTab="5"/>
+    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="119">
   <si>
     <t>7148691</t>
   </si>
@@ -378,9 +378,6 @@
   </si>
   <si>
     <t>tgt</t>
-  </si>
-  <si>
-    <t>usedPatterns</t>
   </si>
   <si>
     <t>valid</t>
@@ -818,7 +815,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -832,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
@@ -1067,7 +1064,7 @@
         <v>105</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1159,7 +1156,7 @@
         <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1189,15 +1186,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F2"/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1213,11 +1214,8 @@
       <c r="E1" t="s">
         <v>86</v>
       </c>
-      <c r="F1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1233,11 +1231,8 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1265,7 +1260,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
@@ -1356,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
@@ -1433,7 +1428,7 @@
         <v>109</v>
       </c>
       <c r="X1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y1" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Renamed relation rrmean[Rule*Meaning] to meaning[Rule*Meaning] in FormalAmpersand and meatgrinder
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/AST.xlsx
+++ b/AmpersandData/FormalAmpersand/AST.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\hjo20125\Git\ampersand\ampersandData\FormalAmpersand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\hjo20125\Git\Ampersand\AmpersandData\FormalAmpersand\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" activeTab="2"/>
+    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" firstSheet="6" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>relations~</t>
-  </si>
-  <si>
-    <t>rrmean</t>
   </si>
   <si>
     <t>rrpurpose</t>
@@ -416,6 +413,9 @@
   </si>
   <si>
     <t>term</t>
+  </si>
+  <si>
+    <t>meaning</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -829,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
@@ -853,10 +853,10 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,16 +1055,16 @@
         <v>97</v>
       </c>
       <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1107,7 +1107,7 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>101</v>
@@ -1156,7 +1156,7 @@
         <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1188,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -1260,7 +1260,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
@@ -1298,7 +1298,7 @@
         <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
@@ -1425,16 +1425,16 @@
         <v>81</v>
       </c>
       <c r="W1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y1" t="s">
         <v>84</v>
       </c>
       <c r="Z1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AA1" t="s">
         <v>99</v>
@@ -1452,10 +1452,10 @@
         <v>97</v>
       </c>
       <c r="AF1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AG1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Renamed relation decprps[Rule*PropertyRule] to propertyRule[Rule*PropertyRule] in FormalAmpersand and meatgrinder
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/AST.xlsx
+++ b/AmpersandData/FormalAmpersand/AST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="7668" yWindow="-12" windowWidth="7476" windowHeight="4968" tabRatio="870" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -279,9 +279,6 @@
   </si>
   <si>
     <t>decprR</t>
-  </si>
-  <si>
-    <t>decprps~</t>
   </si>
   <si>
     <t>decpurpose</t>
@@ -416,6 +413,9 @@
   </si>
   <si>
     <t>meaning</t>
+  </si>
+  <si>
+    <t>propertyRule~</t>
   </si>
 </sst>
 </file>
@@ -784,7 +784,7 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
         <v>72</v>
@@ -815,7 +815,7 @@
         <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
         <v>47</v>
@@ -829,7 +829,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
@@ -853,10 +853,10 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -888,7 +888,7 @@
         <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -963,7 +963,7 @@
         <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -992,7 +992,7 @@
         <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1021,7 +1021,7 @@
         <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1052,19 +1052,19 @@
         <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1107,10 +1107,10 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1144,19 +1144,19 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1203,16 +1203,16 @@
         <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1260,10 +1260,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1295,10 +1295,10 @@
         <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
@@ -1313,7 +1313,7 @@
         <v>77</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1351,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,22 +1422,22 @@
         <v>39</v>
       </c>
       <c r="V1" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="W1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB1" t="s">
         <v>74</v>
@@ -1446,16 +1446,16 @@
         <v>73</v>
       </c>
       <c r="AD1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AE1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AF1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AG1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
@@ -1577,10 +1577,10 @@
         <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1612,13 +1612,13 @@
         <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1655,7 +1655,7 @@
         <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>